<commit_message>
Updated ID/GUID attributes and parsing
</commit_message>
<xml_diff>
--- a/erb/Packaging_Resources/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb/Packaging_Resources/Static_Data/Activity_ID_Chart.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWILKE06\Documents\Eclipse_Repos\metroceri\MetroCERI\erb\Packaging_Resources\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59991A8-4F11-4B4D-AAE9-528BB5D613B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFFB205-819F-4E72-A6DD-9CE131E48925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1230" windowWidth="29040" windowHeight="17640" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="84" yWindow="0" windowWidth="12636" windowHeight="12156" activeTab="2" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Assignments" sheetId="1" r:id="rId1"/>
+    <sheet name="Panels" sheetId="2" r:id="rId2"/>
+    <sheet name="Mapping" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="194">
   <si>
     <t>ID</t>
   </si>
@@ -273,6 +275,351 @@
   </si>
   <si>
     <t>Alternative Note Board Activity</t>
+  </si>
+  <si>
+    <t>ERB Main Panels</t>
+  </si>
+  <si>
+    <t>Landing</t>
+  </si>
+  <si>
+    <t>Project Selection</t>
+  </si>
+  <si>
+    <t>Goal Creation</t>
+  </si>
+  <si>
+    <t>Engagement</t>
+  </si>
+  <si>
+    <t>Resource Panels</t>
+  </si>
+  <si>
+    <t>Intro Panels</t>
+  </si>
+  <si>
+    <t>What makes erb different</t>
+  </si>
+  <si>
+    <t>Dynamic Activity Panels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note board </t>
+  </si>
+  <si>
+    <t>Chapter Panel</t>
+  </si>
+  <si>
+    <t>Activity Panel</t>
+  </si>
+  <si>
+    <t>Step Panel</t>
+  </si>
+  <si>
+    <t>Background Panel</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>0003</t>
+  </si>
+  <si>
+    <t>0004</t>
+  </si>
+  <si>
+    <t>00001</t>
+  </si>
+  <si>
+    <t>00002</t>
+  </si>
+  <si>
+    <t>00003</t>
+  </si>
+  <si>
+    <t>00004</t>
+  </si>
+  <si>
+    <t>00005</t>
+  </si>
+  <si>
+    <t>0000001</t>
+  </si>
+  <si>
+    <t>0000002</t>
+  </si>
+  <si>
+    <t>0000003</t>
+  </si>
+  <si>
+    <t>0000004</t>
+  </si>
+  <si>
+    <t>0000005</t>
+  </si>
+  <si>
+    <t>0000006</t>
+  </si>
+  <si>
+    <t>0000007</t>
+  </si>
+  <si>
+    <t>00000001</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>000001</t>
+  </si>
+  <si>
+    <t>000002</t>
+  </si>
+  <si>
+    <t>000003</t>
+  </si>
+  <si>
+    <t>000004</t>
+  </si>
+  <si>
+    <t>000005</t>
+  </si>
+  <si>
+    <t>000006</t>
+  </si>
+  <si>
+    <t>000007</t>
+  </si>
+  <si>
+    <t>000008</t>
+  </si>
+  <si>
+    <t>000009</t>
+  </si>
+  <si>
+    <t>000010</t>
+  </si>
+  <si>
+    <t>000011</t>
+  </si>
+  <si>
+    <t>000012</t>
+  </si>
+  <si>
+    <t>000013</t>
+  </si>
+  <si>
+    <t>000014</t>
+  </si>
+  <si>
+    <t>000015</t>
+  </si>
+  <si>
+    <t>000016</t>
+  </si>
+  <si>
+    <t>000017</t>
+  </si>
+  <si>
+    <t>000018</t>
+  </si>
+  <si>
+    <t>000019</t>
+  </si>
+  <si>
+    <t>000020</t>
+  </si>
+  <si>
+    <t>000021</t>
+  </si>
+  <si>
+    <t>000022</t>
+  </si>
+  <si>
+    <t>000023</t>
+  </si>
+  <si>
+    <t>000024</t>
+  </si>
+  <si>
+    <t>000025</t>
+  </si>
+  <si>
+    <t>000026</t>
+  </si>
+  <si>
+    <t>000027</t>
+  </si>
+  <si>
+    <t>000028</t>
+  </si>
+  <si>
+    <t>000029</t>
+  </si>
+  <si>
+    <t>000039</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>401</t>
+  </si>
+  <si>
+    <t>421</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>301</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>431</t>
+  </si>
+  <si>
+    <t>432</t>
   </si>
 </sst>
 </file>
@@ -296,7 +643,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,8 +698,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -496,11 +849,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -584,12 +1003,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -613,6 +1026,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -939,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E334887F-75F3-43E4-AB8B-246C79CAC6C0}">
   <dimension ref="A1:V58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,19 +1415,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="55" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="22"/>
@@ -990,26 +1449,26 @@
       <c r="V1" s="22"/>
     </row>
     <row r="2" spans="1:22" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="53" t="s">
+      <c r="B2" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="51" t="s">
         <v>78</v>
       </c>
       <c r="F2" s="23"/>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="46"/>
+      <c r="H2" s="76"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
@@ -1043,7 +1502,7 @@
       </c>
       <c r="F3" s="23"/>
       <c r="G3" s="44"/>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="47" t="s">
         <v>53</v>
       </c>
       <c r="I3" s="23"/>
@@ -1079,7 +1538,7 @@
       </c>
       <c r="F4" s="23"/>
       <c r="G4" s="40"/>
-      <c r="H4" s="49" t="s">
+      <c r="H4" s="47" t="s">
         <v>58</v>
       </c>
       <c r="I4" s="23"/>
@@ -1115,7 +1574,7 @@
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="41"/>
-      <c r="H5" s="49" t="s">
+      <c r="H5" s="47" t="s">
         <v>54</v>
       </c>
       <c r="I5" s="23"/>
@@ -1149,7 +1608,7 @@
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="42"/>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="47" t="s">
         <v>75</v>
       </c>
       <c r="I6" s="24"/>
@@ -1183,7 +1642,7 @@
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="43"/>
-      <c r="H7" s="49" t="s">
+      <c r="H7" s="47" t="s">
         <v>55</v>
       </c>
       <c r="I7" s="24"/>
@@ -1216,8 +1675,8 @@
         <v>67</v>
       </c>
       <c r="F8" s="24"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="49" t="s">
+      <c r="G8" s="49"/>
+      <c r="H8" s="47" t="s">
         <v>56</v>
       </c>
       <c r="I8" s="24"/>
@@ -1250,8 +1709,8 @@
         <v>68</v>
       </c>
       <c r="F9" s="24"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="50" t="s">
+      <c r="G9" s="50"/>
+      <c r="H9" s="48" t="s">
         <v>77</v>
       </c>
       <c r="I9" s="24"/>
@@ -2771,4 +3230,1391 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AD5C8-E087-42D9-8818-93A09826D8C4}">
+  <dimension ref="A1:H41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.109375" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" customWidth="1"/>
+    <col min="12" max="12" width="86.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.77734375" customWidth="1"/>
+    <col min="14" max="14" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="66" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="61" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="61" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="66" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="66" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="H12" s="58" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="63" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="63" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="63" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="63" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="67"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="67"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="67"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="67"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="67"/>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="67"/>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="67"/>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="67"/>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="67"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="63" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="67"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="63" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="67"/>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="67"/>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="67"/>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C31" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="67"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="67"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C33" s="63" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="67"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C34" s="63" t="s">
+        <v>140</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="67"/>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C35" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="67"/>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C36" s="63" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="67"/>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C37" s="63" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="67"/>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C38" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="67"/>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C39" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="67"/>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C40" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="67"/>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C41" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="67"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C403D9B-4156-4D53-B432-05D214EB9E6F}">
+  <dimension ref="A1:K42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" style="24" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" style="24" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="70"/>
+      <c r="D1" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="70"/>
+      <c r="G1" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="70"/>
+      <c r="J1" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="69" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="72"/>
+      <c r="D2" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="72"/>
+      <c r="G2" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="72"/>
+      <c r="J2" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="71" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="72"/>
+      <c r="D3" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="72"/>
+      <c r="G3" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="71" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3" s="72"/>
+      <c r="J3" s="71" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="72"/>
+      <c r="D4" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="72"/>
+      <c r="G4" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="71" t="s">
+        <v>148</v>
+      </c>
+      <c r="I4" s="72"/>
+      <c r="J4" s="71" t="s">
+        <v>100</v>
+      </c>
+      <c r="K4" s="71" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="72"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="71" t="s">
+        <v>148</v>
+      </c>
+      <c r="I5" s="72"/>
+      <c r="J5" s="71" t="s">
+        <v>101</v>
+      </c>
+      <c r="K5" s="71" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="72"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="72"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="72"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="73"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="73"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="70"/>
+      <c r="D11" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="70"/>
+      <c r="G11" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="70"/>
+      <c r="J11" s="68" t="s">
+        <v>117</v>
+      </c>
+      <c r="K11" s="69" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="72"/>
+      <c r="D12" s="71" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="71" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" s="72"/>
+      <c r="G12" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" s="71" t="s">
+        <v>188</v>
+      </c>
+      <c r="I12" s="72"/>
+      <c r="J12" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="K12" s="71" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="72"/>
+      <c r="D13" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="71" t="s">
+        <v>159</v>
+      </c>
+      <c r="F13" s="72"/>
+      <c r="G13" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="H13" s="71" t="s">
+        <v>189</v>
+      </c>
+      <c r="I13" s="72"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="71" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="72"/>
+      <c r="D14" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="71" t="s">
+        <v>160</v>
+      </c>
+      <c r="F14" s="72"/>
+      <c r="G14" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="71" t="s">
+        <v>190</v>
+      </c>
+      <c r="I14" s="72"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="73"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="71" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="71" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="72"/>
+      <c r="D15" s="71" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="71" t="s">
+        <v>161</v>
+      </c>
+      <c r="F15" s="72"/>
+      <c r="G15" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="H15" s="71" t="s">
+        <v>191</v>
+      </c>
+      <c r="I15" s="72"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="71" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="71" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="72"/>
+      <c r="D16" s="71" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="F16" s="72"/>
+      <c r="G16" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="71" t="s">
+        <v>174</v>
+      </c>
+      <c r="I16" s="72"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="73"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="71" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" s="71" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" s="72"/>
+      <c r="G17" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" s="71" t="s">
+        <v>192</v>
+      </c>
+      <c r="I17" s="72"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="73"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="71" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="71" t="s">
+        <v>164</v>
+      </c>
+      <c r="F18" s="72"/>
+      <c r="G18" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="H18" s="71" t="s">
+        <v>193</v>
+      </c>
+      <c r="I18" s="72"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="73"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="71" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" s="71" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="72"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="73"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="71" t="s">
+        <v>166</v>
+      </c>
+      <c r="F20" s="72"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="73"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="73"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" s="71" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" s="72"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="73"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="71" t="s">
+        <v>168</v>
+      </c>
+      <c r="F22" s="72"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="73"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="71" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="71" t="s">
+        <v>169</v>
+      </c>
+      <c r="F23" s="72"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="73"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="73"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="71" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="71" t="s">
+        <v>170</v>
+      </c>
+      <c r="F24" s="72"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="73"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="71" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" s="72"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="73"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="71" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="F26" s="72"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="73"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="73"/>
+      <c r="B27" s="73"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="71" t="s">
+        <v>173</v>
+      </c>
+      <c r="F27" s="72"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="73"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="73"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="73"/>
+      <c r="B28" s="73"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="71" t="s">
+        <v>134</v>
+      </c>
+      <c r="E28" s="71" t="s">
+        <v>175</v>
+      </c>
+      <c r="F28" s="72"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="73"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="73"/>
+      <c r="B29" s="73"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="71" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29" s="72"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="73"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="73"/>
+      <c r="K29" s="73"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="73"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="71" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" s="71" t="s">
+        <v>177</v>
+      </c>
+      <c r="F30" s="72"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="73"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="73"/>
+      <c r="K30" s="73"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="73"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="71" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="71" t="s">
+        <v>178</v>
+      </c>
+      <c r="F31" s="72"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="73"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="73"/>
+      <c r="K31" s="73"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="73"/>
+      <c r="B32" s="73"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" s="71" t="s">
+        <v>179</v>
+      </c>
+      <c r="F32" s="72"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="73"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="73"/>
+      <c r="K32" s="73"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="73"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" s="71" t="s">
+        <v>180</v>
+      </c>
+      <c r="F33" s="72"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="73"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="73"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="73"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="F34" s="72"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="73"/>
+      <c r="B35" s="73"/>
+      <c r="C35" s="74"/>
+      <c r="D35" s="71" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="71" t="s">
+        <v>182</v>
+      </c>
+      <c r="F35" s="72"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="73"/>
+      <c r="I35" s="74"/>
+      <c r="J35" s="73"/>
+      <c r="K35" s="73"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="73"/>
+      <c r="B36" s="73"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="71" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36" s="71" t="s">
+        <v>183</v>
+      </c>
+      <c r="F36" s="72"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="73"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="73"/>
+      <c r="K36" s="73"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="73"/>
+      <c r="B37" s="73"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="71" t="s">
+        <v>184</v>
+      </c>
+      <c r="F37" s="72"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="73"/>
+      <c r="I37" s="74"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="73"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="73"/>
+      <c r="B38" s="73"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="71" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" s="71" t="s">
+        <v>185</v>
+      </c>
+      <c r="F38" s="72"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="73"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="73"/>
+      <c r="B39" s="73"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="E39" s="71" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" s="72"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="73"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="73"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="73"/>
+      <c r="B40" s="73"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="71" t="s">
+        <v>146</v>
+      </c>
+      <c r="E40" s="71" t="s">
+        <v>187</v>
+      </c>
+      <c r="F40" s="72"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="73"/>
+      <c r="I40" s="74"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="59"/>
+      <c r="B41" s="59"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="59"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="59"/>
+      <c r="K41" s="59"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G42" s="67"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove background panels from tree view
</commit_message>
<xml_diff>
--- a/erb/Packaging_Resources/Static_Data/Activity_ID_Chart.xlsx
+++ b/erb/Packaging_Resources/Static_Data/Activity_ID_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWILKE06\Documents\Eclipse_Repos\metroceri\MetroCERI\erb\Packaging_Resources\Static_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BBEC8E-3306-40A4-8F1C-AB0B540AEC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9160BF-963E-4238-BF53-C2D836C009B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="84" yWindow="0" windowWidth="18564" windowHeight="12156" activeTab="1" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
@@ -3236,7 +3236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AD5C8-E087-42D9-8818-93A09826D8C4}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>